<commit_message>
v1.2 - change to Pi built-in headphone jack
v1.2 - change to Pi built-in headphone jack
</commit_message>
<xml_diff>
--- a/case/dqmusicbox.xlsx
+++ b/case/dqmusicbox.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ross\OneDrive\Documents\projects\dqmusicbox\case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\OneDrive\Documents\projects\dqmusicbox\case\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14232" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14230" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="7" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="cherry3" sheetId="26" r:id="rId4"/>
     <sheet name="maple5" sheetId="27" r:id="rId5"/>
     <sheet name="birch5" sheetId="31" r:id="rId6"/>
+    <sheet name="birch6" sheetId="32" r:id="rId7"/>
+    <sheet name="birch7" sheetId="33" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="65">
   <si>
     <t>width</t>
   </si>
@@ -221,6 +223,9 @@
   </si>
   <si>
     <t>birch5</t>
+  </si>
+  <si>
+    <t>birch6</t>
   </si>
 </sst>
 </file>
@@ -620,37 +625,37 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -669,35 +674,35 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -707,7 +712,7 @@
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -715,7 +720,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -723,7 +728,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -731,7 +736,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -739,7 +744,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -768,7 +773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -785,7 +790,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -796,7 +801,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -833,7 +838,7 @@
         <v>125.83</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -868,7 +873,7 @@
         <v>148.005</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -905,7 +910,7 @@
         <v>125.83</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -940,7 +945,7 @@
         <v>145.405</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -976,17 +981,17 @@
         <v>126.58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
@@ -1005,7 +1010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1029,7 +1034,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1040,7 +1045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1060,7 +1065,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1087,7 +1092,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1114,7 +1119,7 @@
         <v>118.854</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1143,7 +1148,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1172,7 +1177,7 @@
         <v>118.854</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1201,7 +1206,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1230,7 +1235,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>21</v>
       </c>
@@ -1247,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1258,7 +1263,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1275,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -1281,7 +1286,7 @@
         <v>67.001000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>50.127000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1315,7 +1320,7 @@
         <v>16.6265</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1323,7 +1328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1336,7 +1341,7 @@
         <v>16.6265</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>19</v>
       </c>
@@ -1352,7 +1357,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>20</v>
       </c>
@@ -1371,7 +1376,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
@@ -1384,7 +1389,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>37</v>
       </c>
@@ -1400,7 +1405,7 @@
         <v>75.132000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
@@ -1416,7 +1421,7 @@
         <v>60.132000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
@@ -1432,7 +1437,7 @@
         <v>45.132000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
@@ -1448,7 +1453,7 @@
         <v>30.132000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
@@ -1464,10 +1469,10 @@
         <v>15.132000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
     </row>
-    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>51</v>
       </c>
@@ -1483,7 +1488,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -1502,7 +1507,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>56</v>
       </c>
@@ -1515,7 +1520,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -1535,7 +1540,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>52</v>
       </c>
@@ -1551,7 +1556,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>50</v>
       </c>
@@ -1584,35 +1589,35 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1622,7 +1627,7 @@
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1630,7 +1635,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1638,7 +1643,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1646,7 +1651,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1654,7 +1659,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -1683,7 +1688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1700,7 +1705,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1711,7 +1716,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1748,7 +1753,7 @@
         <v>125.83</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1783,7 +1788,7 @@
         <v>148.005</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1825,7 @@
         <v>125.83</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1855,7 +1860,7 @@
         <v>145.405</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1891,17 +1896,17 @@
         <v>126.58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
@@ -1920,7 +1925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1931,7 +1936,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1944,7 +1949,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1955,7 +1960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1975,7 +1980,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2002,7 +2007,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -2029,7 +2034,7 @@
         <v>118.854</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2058,7 +2063,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2087,7 +2092,7 @@
         <v>118.854</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -2116,7 +2121,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2145,7 +2150,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>21</v>
       </c>
@@ -2162,7 +2167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2173,7 +2178,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2185,7 +2190,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -2196,7 +2201,7 @@
         <v>67.001000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2209,7 +2214,7 @@
         <v>50.127000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>16.6265</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -2238,7 +2243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -2251,7 +2256,7 @@
         <v>16.6265</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>19</v>
       </c>
@@ -2267,7 +2272,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>20</v>
       </c>
@@ -2286,7 +2291,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
@@ -2299,7 +2304,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>37</v>
       </c>
@@ -2315,7 +2320,7 @@
         <v>75.132000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
@@ -2331,7 +2336,7 @@
         <v>60.132000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>46</v>
       </c>
@@ -2347,7 +2352,7 @@
         <v>45.132000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
@@ -2363,7 +2368,7 @@
         <v>30.132000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
@@ -2379,10 +2384,10 @@
         <v>15.132000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
     </row>
-    <row r="54" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>51</v>
       </c>
@@ -2398,7 +2403,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -2417,7 +2422,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>56</v>
       </c>
@@ -2430,7 +2435,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>57</v>
       </c>
@@ -2450,7 +2455,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>52</v>
       </c>
@@ -2466,7 +2471,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>50</v>
       </c>
@@ -2499,35 +2504,35 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -2537,7 +2542,7 @@
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2545,7 +2550,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2553,7 +2558,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2569,7 +2574,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -2598,7 +2603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2615,7 +2620,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2626,7 +2631,7 @@
         <v>66.254000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2663,7 +2668,7 @@
         <v>124.48649999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2700,7 +2705,7 @@
         <v>126.074</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2735,7 +2740,7 @@
         <v>146.249</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -2772,7 +2777,7 @@
         <v>126.074</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2807,7 +2812,7 @@
         <v>144.249</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2843,17 +2848,17 @@
         <v>126.79899999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>13</v>
       </c>
@@ -2872,7 +2877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2883,7 +2888,7 @@
         <v>96.122</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2896,7 +2901,7 @@
         <v>66.254000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -2907,7 +2912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -2927,7 +2932,7 @@
         <v>105.122</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>106.122</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2981,7 +2986,7 @@
         <v>118.976</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -3010,7 +3015,7 @@
         <v>106.122</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3039,7 +3044,7 @@
         <v>118.976</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -3068,7 +3073,7 @@
         <v>106.122</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>106.122</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
@@ -3114,7 +3119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -3125,7 +3130,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -3137,7 +3142,7 @@
         <v>90.254000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>67.001000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -3161,7 +3166,7 @@
         <v>50.249000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -3182,7 +3187,7 @@
         <v>16.7485</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -3190,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -3203,7 +3208,7 @@
         <v>16.7485</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>19</v>
       </c>
@@ -3219,7 +3224,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>20</v>
       </c>
@@ -3238,7 +3243,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
@@ -3251,7 +3256,7 @@
         <v>90.254000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>37</v>
       </c>
@@ -3267,7 +3272,7 @@
         <v>75.376000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
@@ -3283,7 +3288,7 @@
         <v>60.376000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
@@ -3299,7 +3304,7 @@
         <v>45.376000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
@@ -3315,7 +3320,7 @@
         <v>30.376000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
@@ -3331,7 +3336,7 @@
         <v>15.376000000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>51</v>
       </c>
@@ -3347,7 +3352,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>163.12200000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>52</v>
       </c>
@@ -3382,7 +3387,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>50</v>
       </c>
@@ -3415,35 +3420,35 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -3453,7 +3458,7 @@
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3461,7 +3466,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3469,7 +3474,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -3477,7 +3482,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -3485,7 +3490,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3532,7 +3537,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3543,7 +3548,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -3580,7 +3585,7 @@
         <v>420.24250000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -3617,7 +3622,7 @@
         <v>421.83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -3652,7 +3657,7 @@
         <v>442.005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -3689,7 +3694,7 @@
         <v>421.83</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -3724,7 +3729,7 @@
         <v>440.005</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3760,17 +3765,17 @@
         <v>422.58</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>13</v>
       </c>
@@ -3789,7 +3794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -3801,7 +3806,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -3812,7 +3817,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -3823,7 +3828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -3843,7 +3848,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3870,7 +3875,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -3897,7 +3902,7 @@
         <v>414.85399999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -3926,7 +3931,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3955,7 +3960,7 @@
         <v>414.85399999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -3984,7 +3989,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -4013,7 +4018,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
@@ -4030,7 +4035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -4041,7 +4046,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -4052,7 +4057,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -4063,7 +4068,7 @@
         <v>67.001000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -4076,7 +4081,7 @@
         <v>346.005</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -4097,7 +4102,7 @@
         <v>312.50450000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -4105,7 +4110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -4118,7 +4123,7 @@
         <v>312.50450000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>19</v>
       </c>
@@ -4134,7 +4139,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>20</v>
       </c>
@@ -4153,7 +4158,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
@@ -4166,7 +4171,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>37</v>
       </c>
@@ -4182,7 +4187,7 @@
         <v>371.01</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
@@ -4198,7 +4203,7 @@
         <v>356.01</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
@@ -4214,7 +4219,7 @@
         <v>341.01</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
@@ -4230,7 +4235,7 @@
         <v>326.01</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
@@ -4246,7 +4251,7 @@
         <v>311.01</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>51</v>
       </c>
@@ -4262,7 +4267,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -4282,7 +4287,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>52</v>
       </c>
@@ -4298,7 +4303,7 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>50</v>
       </c>
@@ -4329,39 +4334,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="81.44140625" customWidth="1"/>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -4371,7 +4376,7 @@
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4379,7 +4384,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -4387,7 +4392,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -4395,7 +4400,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -4403,7 +4408,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -4432,7 +4437,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -4449,7 +4454,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -4460,7 +4465,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -4497,7 +4502,7 @@
         <v>124.24249999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -4510,11 +4515,11 @@
         <v>33.005000000000003</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D19" si="0">B15+$B$12</f>
+        <f t="shared" ref="D15:D18" si="0">B15+$B$12</f>
         <v>65.12533333333333</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" ref="E15:E19" si="1">C15+$C$12</f>
+        <f t="shared" ref="E15:E18" si="1">C15+$C$12</f>
         <v>129.005</v>
       </c>
       <c r="F15">
@@ -4534,7 +4539,7 @@
         <v>125.83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -4569,7 +4574,7 @@
         <v>148.005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -4606,7 +4611,7 @@
         <v>125.83</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4641,7 +4646,7 @@
         <v>145.405</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -4677,17 +4682,17 @@
         <v>126.58</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>13</v>
       </c>
@@ -4706,7 +4711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -4717,7 +4722,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -4730,7 +4735,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -4741,7 +4746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -4761,7 +4766,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -4788,7 +4793,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -4815,7 +4820,7 @@
         <v>118.854</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -4844,7 +4849,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -4873,7 +4878,7 @@
         <v>118.854</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -4902,7 +4907,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -4931,7 +4936,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
@@ -4948,7 +4953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -4959,7 +4964,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -4971,7 +4976,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -4982,7 +4987,7 @@
         <v>67.001000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -4995,7 +5000,7 @@
         <v>50.127000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -5016,7 +5021,7 @@
         <v>16.6265</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -5024,7 +5029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -5037,7 +5042,7 @@
         <v>16.6265</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>19</v>
       </c>
@@ -5053,7 +5058,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>20</v>
       </c>
@@ -5072,7 +5077,7 @@
         <v>5.1219999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
@@ -5085,7 +5090,7 @@
         <v>90.01</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>37</v>
       </c>
@@ -5101,7 +5106,7 @@
         <v>75.132000000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
@@ -5117,7 +5122,7 @@
         <v>60.132000000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>46</v>
       </c>
@@ -5133,7 +5138,7 @@
         <v>45.132000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>48</v>
       </c>
@@ -5149,7 +5154,7 @@
         <v>30.132000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
@@ -5165,10 +5170,10 @@
         <v>15.132000000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
     </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>51</v>
       </c>
@@ -5184,7 +5189,7 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>53</v>
       </c>
@@ -5203,7 +5208,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>56</v>
       </c>
@@ -5216,7 +5221,7 @@
         <v>66.010000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
@@ -5236,7 +5241,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A61" s="8" t="s">
         <v>52</v>
       </c>
@@ -5252,7 +5257,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>50</v>
       </c>
@@ -5269,6 +5274,1890 @@
       <c r="I62">
         <f>C62</f>
         <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="C12">
+        <v>96</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>180.01</v>
+      </c>
+      <c r="C13">
+        <v>66.010000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <f>B13/8</f>
+        <v>22.501249999999999</v>
+      </c>
+      <c r="C14">
+        <f>C13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D14">
+        <f>B14+B12</f>
+        <v>27.623249999999999</v>
+      </c>
+      <c r="E14">
+        <f>C14+C12</f>
+        <v>129.005</v>
+      </c>
+      <c r="F14">
+        <f>(3/8)*25.4</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="G14">
+        <f>F14</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="H14">
+        <f>D14-(F14/2)</f>
+        <v>22.860749999999999</v>
+      </c>
+      <c r="I14">
+        <f>E14-(G14/2)</f>
+        <v>124.24249999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f>$B$13/3</f>
+        <v>60.00333333333333</v>
+      </c>
+      <c r="C15" s="4">
+        <f>$C$13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D18" si="0">B15+$B$12</f>
+        <v>65.12533333333333</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" ref="E15:E18" si="1">C15+$C$12</f>
+        <v>129.005</v>
+      </c>
+      <c r="F15">
+        <f>(1/4)*25.4</f>
+        <v>6.35</v>
+      </c>
+      <c r="G15">
+        <f>F15</f>
+        <v>6.35</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:I19" si="2">D15-(F15/2)</f>
+        <v>61.950333333333333</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>125.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <f>B15</f>
+        <v>60.00333333333333</v>
+      </c>
+      <c r="C16" s="4">
+        <f>$C$13/2+21</f>
+        <v>54.005000000000003</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>65.12533333333333</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>150.005</v>
+      </c>
+      <c r="F16">
+        <v>36.972000000000001</v>
+      </c>
+      <c r="G16">
+        <v>7.9980000000000002</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>46.639333333333326</v>
+      </c>
+      <c r="I16">
+        <f>E16-(G16/2)+2</f>
+        <v>148.006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f>$B$13/3*2</f>
+        <v>120.00666666666666</v>
+      </c>
+      <c r="C17" s="4">
+        <f>$C$13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>125.12866666666666</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
+        <v>129.005</v>
+      </c>
+      <c r="F17">
+        <f>(1/4)*25.4</f>
+        <v>6.35</v>
+      </c>
+      <c r="G17">
+        <f>F17</f>
+        <v>6.35</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>121.95366666666666</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>125.83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f>$B$13/3*2</f>
+        <v>120.00666666666666</v>
+      </c>
+      <c r="C18" s="4">
+        <f>$C$13/2+21</f>
+        <v>54.005000000000003</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>125.12866666666666</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>150.005</v>
+      </c>
+      <c r="F18">
+        <v>29.280999999999999</v>
+      </c>
+      <c r="G18">
+        <v>7.9980000000000002</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>110.48816666666666</v>
+      </c>
+      <c r="I18">
+        <f>E18-(G18/2)-2.6+2</f>
+        <v>145.40600000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <f>B13/8*7</f>
+        <v>157.50874999999999</v>
+      </c>
+      <c r="C19" s="4">
+        <f>C13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D19">
+        <f>B19+B12</f>
+        <v>162.63074999999998</v>
+      </c>
+      <c r="E19" s="4">
+        <f>C19+C12</f>
+        <v>129.005</v>
+      </c>
+      <c r="F19">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G19">
+        <f>F19</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>160.20574999999997</v>
+      </c>
+      <c r="I19">
+        <f>E19-(G19/2)</f>
+        <v>126.58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>186.12200000000001</v>
+      </c>
+      <c r="C23">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <f>B13</f>
+        <v>180.01</v>
+      </c>
+      <c r="C24">
+        <f>C13</f>
+        <v>66.010000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <f>B24-(B25*2)</f>
+        <v>162.01</v>
+      </c>
+      <c r="G26">
+        <v>32</v>
+      </c>
+      <c r="H26">
+        <f>B23+B25</f>
+        <v>195.12200000000001</v>
+      </c>
+      <c r="I26">
+        <f>C23+C25</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <f>H27+(F27/2)</f>
+        <v>211.12200000000001</v>
+      </c>
+      <c r="C27">
+        <f>I27+(G27/2)</f>
+        <v>121</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27">
+        <v>30</v>
+      </c>
+      <c r="H27">
+        <f>H26+1</f>
+        <v>196.12200000000001</v>
+      </c>
+      <c r="I27">
+        <f>I26+1</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <f>B27</f>
+        <v>211.12200000000001</v>
+      </c>
+      <c r="C28">
+        <f>C27</f>
+        <v>121</v>
+      </c>
+      <c r="F28">
+        <v>5.85</v>
+      </c>
+      <c r="G28">
+        <v>4.2919999999999998</v>
+      </c>
+      <c r="H28">
+        <f>B28-(F28/2)</f>
+        <v>208.197</v>
+      </c>
+      <c r="I28">
+        <f>C28-(G28/2)</f>
+        <v>118.854</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <f>B28+F29+1</f>
+        <v>242.12200000000001</v>
+      </c>
+      <c r="C29">
+        <f>C27</f>
+        <v>121</v>
+      </c>
+      <c r="F29">
+        <f>F27</f>
+        <v>30</v>
+      </c>
+      <c r="G29">
+        <f>G27</f>
+        <v>30</v>
+      </c>
+      <c r="H29">
+        <f>B29-(F29/2)</f>
+        <v>227.12200000000001</v>
+      </c>
+      <c r="I29">
+        <f>I27</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <f>B29</f>
+        <v>242.12200000000001</v>
+      </c>
+      <c r="C30">
+        <f>C29</f>
+        <v>121</v>
+      </c>
+      <c r="F30">
+        <f>F28</f>
+        <v>5.85</v>
+      </c>
+      <c r="G30">
+        <f>G28</f>
+        <v>4.2919999999999998</v>
+      </c>
+      <c r="H30">
+        <f>B30-(F30/2)</f>
+        <v>239.197</v>
+      </c>
+      <c r="I30">
+        <f>C30-(G30/2)</f>
+        <v>118.854</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <f>B29+F31+1</f>
+        <v>273.12200000000001</v>
+      </c>
+      <c r="C31">
+        <f>C27</f>
+        <v>121</v>
+      </c>
+      <c r="F31">
+        <f>F27</f>
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <f>G27</f>
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <f>B31-(F31/2)</f>
+        <v>258.12200000000001</v>
+      </c>
+      <c r="I31">
+        <f>C31-(G31/2)</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <f>B31+F32+1</f>
+        <v>304.12200000000001</v>
+      </c>
+      <c r="C32">
+        <f>C27</f>
+        <v>121</v>
+      </c>
+      <c r="F32">
+        <f>F27</f>
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <f>G27</f>
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <f>B32-(F32/2)</f>
+        <v>289.12200000000001</v>
+      </c>
+      <c r="I32">
+        <f>C32-(G32/2)</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="C36">
+        <v>5.1219999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <f>B24</f>
+        <v>180.01</v>
+      </c>
+      <c r="C37">
+        <v>90.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38">
+        <v>50.648000000000003</v>
+      </c>
+      <c r="C38">
+        <v>67.001000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f>B36+(B37/2)</f>
+        <v>95.126999999999995</v>
+      </c>
+      <c r="C39">
+        <f>C36+(C37/2)</f>
+        <v>50.127000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40">
+        <f>B39-(B38/2)</f>
+        <v>69.802999999999997</v>
+      </c>
+      <c r="C40">
+        <f>C39-(C38/2)</f>
+        <v>16.6265</v>
+      </c>
+      <c r="H40">
+        <f>B39-(B38/2)</f>
+        <v>69.802999999999997</v>
+      </c>
+      <c r="I40">
+        <f>C39-(C38/2)</f>
+        <v>16.6265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <f>H40-B41</f>
+        <v>62.802999999999997</v>
+      </c>
+      <c r="I42">
+        <f>I40</f>
+        <v>16.6265</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>186</v>
+      </c>
+      <c r="C46">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="H46">
+        <f>B46</f>
+        <v>186</v>
+      </c>
+      <c r="I46">
+        <f>C46</f>
+        <v>5.1219999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <f>B37</f>
+        <v>180.01</v>
+      </c>
+      <c r="C47">
+        <f>C37</f>
+        <v>90.01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G48">
+        <v>6</v>
+      </c>
+      <c r="H48">
+        <f>B46+15</f>
+        <v>201</v>
+      </c>
+      <c r="I48">
+        <f>I46+C47-20</f>
+        <v>75.132000000000005</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <f>H48</f>
+        <v>201</v>
+      </c>
+      <c r="I49">
+        <f>I48-15</f>
+        <v>60.132000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <f>H48</f>
+        <v>201</v>
+      </c>
+      <c r="I50">
+        <f>I49-15</f>
+        <v>45.132000000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <f>H48</f>
+        <v>201</v>
+      </c>
+      <c r="I51">
+        <f>I50-15</f>
+        <v>30.132000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <f>H48</f>
+        <v>201</v>
+      </c>
+      <c r="I52">
+        <f>I51-15</f>
+        <v>15.132000000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="55" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A55" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="C56">
+        <v>163</v>
+      </c>
+      <c r="H56">
+        <f>B56</f>
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="I56">
+        <f>C56</f>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f>C37</f>
+        <v>90.01</v>
+      </c>
+      <c r="C57">
+        <f>C24</f>
+        <v>66.010000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58">
+        <v>6</v>
+      </c>
+      <c r="G58">
+        <f>C57-15-B8</f>
+        <v>45.81</v>
+      </c>
+      <c r="H58">
+        <f>H56+45-(F58/2)</f>
+        <v>47.122</v>
+      </c>
+      <c r="I58">
+        <f>I56+15</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A61" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62">
+        <v>96</v>
+      </c>
+      <c r="C62">
+        <v>163</v>
+      </c>
+      <c r="H62">
+        <f>B62</f>
+        <v>96</v>
+      </c>
+      <c r="I62">
+        <f>C62</f>
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="76.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.08984375" customWidth="1"/>
+    <col min="6" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="10" max="10" width="81.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>108</v>
+      </c>
+      <c r="C12">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>180.01</v>
+      </c>
+      <c r="C13">
+        <v>66.010000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <f>B13/8</f>
+        <v>22.501249999999999</v>
+      </c>
+      <c r="C14">
+        <f>C13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D14">
+        <f>B14+B12</f>
+        <v>130.50125</v>
+      </c>
+      <c r="E14">
+        <f>C14+C12</f>
+        <v>38.127000000000002</v>
+      </c>
+      <c r="F14">
+        <f>(3/8)*25.4</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="G14">
+        <f>F14</f>
+        <v>9.5249999999999986</v>
+      </c>
+      <c r="H14">
+        <f>D14-(F14/2)</f>
+        <v>125.73875</v>
+      </c>
+      <c r="I14">
+        <f>E14-(G14/2)</f>
+        <v>33.364500000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f>$B$13/3</f>
+        <v>60.00333333333333</v>
+      </c>
+      <c r="C15" s="4">
+        <f>$C$13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D18" si="0">B15+$B$12</f>
+        <v>168.00333333333333</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" ref="E15:E18" si="1">C15+$C$12</f>
+        <v>38.127000000000002</v>
+      </c>
+      <c r="F15">
+        <f>(1/4)*25.4</f>
+        <v>6.35</v>
+      </c>
+      <c r="G15">
+        <f>F15</f>
+        <v>6.35</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:I19" si="2">D15-(F15/2)</f>
+        <v>164.82833333333332</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>34.952000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <f>B15</f>
+        <v>60.00333333333333</v>
+      </c>
+      <c r="C16" s="4">
+        <f>$C$13/2+21</f>
+        <v>54.005000000000003</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>168.00333333333333</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>59.127000000000002</v>
+      </c>
+      <c r="F16">
+        <v>36.972000000000001</v>
+      </c>
+      <c r="G16">
+        <v>7.9980000000000002</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>149.51733333333334</v>
+      </c>
+      <c r="I16">
+        <f>E16-(G16/2)+2</f>
+        <v>57.128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f>$B$13/3*2</f>
+        <v>120.00666666666666</v>
+      </c>
+      <c r="C17" s="4">
+        <f>$C$13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>228.00666666666666</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
+        <v>38.127000000000002</v>
+      </c>
+      <c r="F17">
+        <f>(1/4)*25.4</f>
+        <v>6.35</v>
+      </c>
+      <c r="G17">
+        <f>F17</f>
+        <v>6.35</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>224.83166666666665</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>34.952000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f>$B$13/3*2</f>
+        <v>120.00666666666666</v>
+      </c>
+      <c r="C18" s="4">
+        <f>$C$13/2+21</f>
+        <v>54.005000000000003</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>228.00666666666666</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="1"/>
+        <v>59.127000000000002</v>
+      </c>
+      <c r="F18">
+        <v>29.280999999999999</v>
+      </c>
+      <c r="G18">
+        <v>7.9980000000000002</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>213.36616666666666</v>
+      </c>
+      <c r="I18">
+        <f>E18-(G18/2)-2.6+2</f>
+        <v>54.527999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <f>B13/8*7</f>
+        <v>157.50874999999999</v>
+      </c>
+      <c r="C19" s="4">
+        <f>C13/2</f>
+        <v>33.005000000000003</v>
+      </c>
+      <c r="D19">
+        <f>B19+B12</f>
+        <v>265.50874999999996</v>
+      </c>
+      <c r="E19" s="4">
+        <f>C19+C12</f>
+        <v>38.127000000000002</v>
+      </c>
+      <c r="F19">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="G19">
+        <f>F19</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>263.08374999999995</v>
+      </c>
+      <c r="I19">
+        <f>E19-(G19/2)</f>
+        <v>35.702000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C20" s="4"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>108</v>
+      </c>
+      <c r="C23">
+        <v>150.78899999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <f>B13</f>
+        <v>180.01</v>
+      </c>
+      <c r="C24">
+        <f>C13</f>
+        <v>66.010000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <f>B24-(B25*2)</f>
+        <v>162.01</v>
+      </c>
+      <c r="G26">
+        <v>32</v>
+      </c>
+      <c r="H26">
+        <f>B23+B25</f>
+        <v>117</v>
+      </c>
+      <c r="I26">
+        <f>C23+C25</f>
+        <v>159.78899999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <f>H27+(F27/2)</f>
+        <v>133</v>
+      </c>
+      <c r="C27">
+        <f>I27+(G27/2)</f>
+        <v>175.78899999999999</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27">
+        <v>30</v>
+      </c>
+      <c r="H27">
+        <f>H26+1</f>
+        <v>118</v>
+      </c>
+      <c r="I27">
+        <f>I26+1</f>
+        <v>160.78899999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <f>B27</f>
+        <v>133</v>
+      </c>
+      <c r="C28">
+        <f>C27</f>
+        <v>175.78899999999999</v>
+      </c>
+      <c r="F28">
+        <v>5.85</v>
+      </c>
+      <c r="G28">
+        <v>4.2919999999999998</v>
+      </c>
+      <c r="H28">
+        <f>B28-(F28/2)</f>
+        <v>130.07499999999999</v>
+      </c>
+      <c r="I28">
+        <f>C28-(G28/2)</f>
+        <v>173.643</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <f>B28+F29+1</f>
+        <v>164</v>
+      </c>
+      <c r="C29">
+        <f>C27</f>
+        <v>175.78899999999999</v>
+      </c>
+      <c r="F29">
+        <f>F27</f>
+        <v>30</v>
+      </c>
+      <c r="G29">
+        <f>G27</f>
+        <v>30</v>
+      </c>
+      <c r="H29">
+        <f>B29-(F29/2)</f>
+        <v>149</v>
+      </c>
+      <c r="I29">
+        <f>I27</f>
+        <v>160.78899999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <f>B29</f>
+        <v>164</v>
+      </c>
+      <c r="C30">
+        <f>C29</f>
+        <v>175.78899999999999</v>
+      </c>
+      <c r="F30">
+        <f>F28</f>
+        <v>5.85</v>
+      </c>
+      <c r="G30">
+        <f>G28</f>
+        <v>4.2919999999999998</v>
+      </c>
+      <c r="H30">
+        <f>B30-(F30/2)</f>
+        <v>161.07499999999999</v>
+      </c>
+      <c r="I30">
+        <f>C30-(G30/2)</f>
+        <v>173.643</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31">
+        <f>B29+F31+1</f>
+        <v>195</v>
+      </c>
+      <c r="C31">
+        <f>C27</f>
+        <v>175.78899999999999</v>
+      </c>
+      <c r="F31">
+        <f>F27</f>
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <f>G27</f>
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <f>B31-(F31/2)</f>
+        <v>180</v>
+      </c>
+      <c r="I31">
+        <f>C31-(G31/2)</f>
+        <v>160.78899999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <f>B31+F32+1</f>
+        <v>226</v>
+      </c>
+      <c r="C32">
+        <f>C27</f>
+        <v>175.78899999999999</v>
+      </c>
+      <c r="F32">
+        <f>F27</f>
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <f>G27</f>
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <f>B32-(F32/2)</f>
+        <v>211</v>
+      </c>
+      <c r="I32">
+        <f>C32-(G32/2)</f>
+        <v>160.78899999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36">
+        <v>108</v>
+      </c>
+      <c r="C36">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <f>B24</f>
+        <v>180.01</v>
+      </c>
+      <c r="C37">
+        <v>90.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38">
+        <v>50.648000000000003</v>
+      </c>
+      <c r="C38">
+        <v>67.001000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f>B36+(B37/2)</f>
+        <v>198.005</v>
+      </c>
+      <c r="C39">
+        <f>C36+(C37/2)</f>
+        <v>111.005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40">
+        <f>B39-(B38/2)</f>
+        <v>172.68099999999998</v>
+      </c>
+      <c r="C40">
+        <f>C39-(C38/2)</f>
+        <v>77.504499999999993</v>
+      </c>
+      <c r="H40">
+        <f>B39-(B38/2)</f>
+        <v>172.68099999999998</v>
+      </c>
+      <c r="I40">
+        <f>C39-(C38/2)</f>
+        <v>77.504499999999993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <f>H40-B41</f>
+        <v>165.68099999999998</v>
+      </c>
+      <c r="I42">
+        <f>I40</f>
+        <v>77.504499999999993</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>108</v>
+      </c>
+      <c r="C46">
+        <v>211.62299999999999</v>
+      </c>
+      <c r="H46">
+        <f>B46</f>
+        <v>108</v>
+      </c>
+      <c r="I46">
+        <f>C46</f>
+        <v>211.62299999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <f>B37</f>
+        <v>180.01</v>
+      </c>
+      <c r="C47">
+        <f>C37</f>
+        <v>90.01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G48">
+        <v>6</v>
+      </c>
+      <c r="H48">
+        <f>B46+(B47/2)-(44.676/2)</f>
+        <v>175.667</v>
+      </c>
+      <c r="I48">
+        <f>I46+C47-20</f>
+        <v>281.63299999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <f>H48</f>
+        <v>175.667</v>
+      </c>
+      <c r="I49">
+        <f>I48-15</f>
+        <v>266.63299999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <f>H48</f>
+        <v>175.667</v>
+      </c>
+      <c r="I50">
+        <f>I49-15</f>
+        <v>251.63299999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <f>H48</f>
+        <v>175.667</v>
+      </c>
+      <c r="I51">
+        <f>I50-15</f>
+        <v>236.63299999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <f>H48</f>
+        <v>175.667</v>
+      </c>
+      <c r="I52">
+        <f>I51-15</f>
+        <v>221.63299999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="55" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A55" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>23.22</v>
+      </c>
+      <c r="C56">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="H56">
+        <f>B56</f>
+        <v>23.22</v>
+      </c>
+      <c r="I56">
+        <f>C56</f>
+        <v>5.1219999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f>C37</f>
+        <v>90.01</v>
+      </c>
+      <c r="C57">
+        <f>C24</f>
+        <v>66.010000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A60" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61">
+        <v>282.81900000000002</v>
+      </c>
+      <c r="C61">
+        <v>5.1219999999999999</v>
+      </c>
+      <c r="H61">
+        <f>B61</f>
+        <v>282.81900000000002</v>
+      </c>
+      <c r="I61">
+        <f>C61</f>
+        <v>5.1219999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>